<commit_message>
Modified to include the simulation metrics in the json file
</commit_message>
<xml_diff>
--- a/Bizagi/simulation_metrics-2.xlsx
+++ b/Bizagi/simulation_metrics-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Data\Bizagi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mclau\source\repos\bizagi_simulations\Bizagi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:9_{9819BCFB-CE32-4F9C-A9CD-BCC0A7554E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16FFA39C-07DA-4D38-A661-22DC4899A92D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9BBE1E-312D-4636-8FD0-3BB4DF67A652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="4185" windowWidth="25815" windowHeight="12030" xr2:uid="{1DFEDFA4-C2BE-44EB-BC93-19389BFEE2AD}"/>
+    <workbookView xWindow="5040" yWindow="1935" windowWidth="25815" windowHeight="12030" xr2:uid="{1DFEDFA4-C2BE-44EB-BC93-19389BFEE2AD}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation_metrics" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>Tech</t>
   </si>
   <si>
-    <t>Complete  /Accurate?</t>
-  </si>
-  <si>
     <t>Gateway</t>
   </si>
   <si>
@@ -105,13 +102,16 @@
   </si>
   <si>
     <t>Start</t>
+  </si>
+  <si>
+    <t>Complete /Accurate?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -968,15 +968,17 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1034,12 +1036,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="H3">
         <v>0.75</v>
@@ -1048,9 +1050,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1071,9 +1073,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1094,12 +1096,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>0.5</v>
@@ -1108,15 +1110,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1131,12 +1133,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
       </c>
       <c r="J8">
         <v>2</v>

</xml_diff>